<commit_message>
Added MCNP results for the 88" Vault simulation
</commit_message>
<xml_diff>
--- a/Simulated/88Inch_Activation/Foils_Cave01.xlsx
+++ b/Simulated/88Inch_Activation/Foils_Cave01.xlsx
@@ -490,7 +490,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="C16" sqref="C16:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -903,10 +903,10 @@
         <v>9</v>
       </c>
       <c r="C16" s="4">
-        <v>511</v>
+        <v>159.38</v>
       </c>
       <c r="D16" s="4">
-        <v>169.6</v>
+        <v>68.3</v>
       </c>
       <c r="E16" s="8">
         <v>51400000000</v>

</xml_diff>